<commit_message>
refactor excess keys (monetary, append, fn) support into support of pre and post function arrays for simplicity and extensibility
</commit_message>
<xml_diff>
--- a/src/tempgen/tests/fixtures/test_template.xlsx
+++ b/src/tempgen/tests/fixtures/test_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Main\Documents\accounting\tests\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Main\Documents\accounting\src\tempgen\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Итого:</t>
   </si>
@@ -48,12 +48,6 @@
     <t xml:space="preserve">Плательщик: {{{"id": "client", "title": "Заказчик", "value": "ООО \"Рога и копыта\""}}}                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                </t>
   </si>
   <si>
-    <t>{{{"id": "total", "title": "Сумма", "value": "2500", "append": " руб.", "monetary": " True"}}}</t>
-  </si>
-  <si>
-    <t>{{{"id": "total", "title": "Сумма", "value": "2500", "fn": "num2text"}}}</t>
-  </si>
-  <si>
     <t>({{{"id": "executive_responsible", "title": "Руководитель предприятия", "value": "ИП Иванов И.И."}}})</t>
   </si>
   <si>
@@ -61,6 +55,15 @@
   </si>
   <si>
     <t>Адрес:  {{{"id": "doer_address", "title": "Адрес", "value": "111111 г.Город, ул. Уличная д.1 к.1 кв.1"}}}</t>
+  </si>
+  <si>
+    <t>{{{"id": "total", "title": "Сумма", "value": "2500", "post": [{"fn": "ru_monetary_string_replace"}, {"fn": "append", "args": [" руб."]}]}}}</t>
+  </si>
+  <si>
+    <t>{{{"id": "total", "title": "Сумма", "value": "2500", "post": [{"fn": "ru_monetary_as_string"}]}}}</t>
+  </si>
+  <si>
+    <t>{{{"id": "total", "title": "Сумма", "value": "2500", "post": [{"fn": "ru_monetary_string_replace"}, {"fn": "append", "args": [" руб."]}]}}}</t>
   </si>
 </sst>
 </file>
@@ -412,9 +415,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -432,6 +432,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -734,7 +737,7 @@
   <dimension ref="B1:BZ122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.1640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -879,15 +882,15 @@
       <c r="BK2"/>
     </row>
     <row r="3" spans="2:63" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
-        <v>13</v>
+      <c r="B3" s="21" t="s">
+        <v>11</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
@@ -1009,14 +1012,14 @@
     </row>
     <row r="5" spans="2:63" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -1200,14 +1203,14 @@
       <c r="BK7"/>
     </row>
     <row r="8" spans="2:63" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="9"/>
       <c r="I8"/>
       <c r="J8"/>
@@ -1340,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1407,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1530,14 +1533,14 @@
     </row>
     <row r="13" spans="2:63" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20" t="s">
-        <v>9</v>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19" t="s">
+        <v>14</v>
       </c>
-      <c r="F13" s="20"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13"/>
@@ -1598,13 +1601,13 @@
     </row>
     <row r="14" spans="2:63" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="16"/>
-      <c r="C14" s="21" t="s">
-        <v>10</v>
+      <c r="C14" s="20" t="s">
+        <v>13</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="16"/>
       <c r="I14"/>
       <c r="J14"/>
@@ -1731,17 +1734,17 @@
       </c>
       <c r="C16" s="3"/>
       <c r="E16" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
@@ -1861,7 +1864,7 @@
       </c>
       <c r="C18" s="3"/>
       <c r="E18" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -9721,7 +9724,6 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B9:G9"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="B8:G8"/>
@@ -9731,6 +9733,7 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B9:G9"/>
   </mergeCells>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1.295275590551181" bottom="1.295275590551181" header="1" footer="1"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>